<commit_message>
Remove Gas Upper Constraint and Add CB3 to A25E65
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_CAP21-A25E65.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_CAP21-A25E65.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1242AFA0-8CA0-40A4-8B61-AA02B0956957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D860A1CA-EC81-4A11-B94A-A0F81EFA7BA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1900,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,19 +1911,18 @@
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="8" customWidth="1"/>
-    <col min="15" max="21" width="9.140625" style="8"/>
-    <col min="22" max="22" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="8"/>
+    <col min="14" max="15" width="16.42578125" style="8" customWidth="1"/>
+    <col min="16" max="22" width="9.140625" style="8"/>
+    <col min="23" max="23" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
       <c r="M1"/>
-      <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
@@ -1936,13 +1934,13 @@
       <c r="X1"/>
       <c r="Y1"/>
       <c r="Z1"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA1"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
       <c r="M2"/>
-      <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
@@ -1954,13 +1952,13 @@
       <c r="X2"/>
       <c r="Y2"/>
       <c r="Z2"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="M3"/>
-      <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3"/>
@@ -1972,8 +1970,9 @@
       <c r="X3"/>
       <c r="Y3"/>
       <c r="Z3"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA3"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" t="s">
         <v>61</v>
@@ -1982,7 +1981,6 @@
         <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","NetZero","CO2","2050")</f>
         <v>UC_NetZero_CO2_2050</v>
       </c>
-      <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
@@ -1994,8 +1992,9 @@
       <c r="X4"/>
       <c r="Y4"/>
       <c r="Z4"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>66</v>
@@ -2004,7 +2003,6 @@
         <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050")</f>
         <v>Net Zero CO2 by 2050</v>
       </c>
-      <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
       <c r="R5"/>
@@ -2016,8 +2014,9 @@
       <c r="X5"/>
       <c r="Y5"/>
       <c r="Z5"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA5"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>72</v>
       </c>
@@ -2055,13 +2054,16 @@
         <v>2030</v>
       </c>
       <c r="N6" s="8">
+        <v>2035</v>
+      </c>
+      <c r="O6" s="8">
         <v>2050</v>
       </c>
-      <c r="O6" s="8">
+      <c r="P6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2099,13 +2101,16 @@
         <v>14093</v>
       </c>
       <c r="N7" s="16">
+        <v>13848.092860693008</v>
+      </c>
+      <c r="O7" s="16">
         <v>0</v>
       </c>
-      <c r="O7" s="8">
+      <c r="P7" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>77</v>
       </c>
@@ -2156,8 +2161,12 @@
         <f t="shared" si="1"/>
         <v>T-A*INT*,T-NAV*</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O8" s="8" t="str">
+        <f>M8</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>62</v>
       </c>
@@ -2208,8 +2217,12 @@
         <f t="shared" si="3"/>
         <v>*CO2*,-*CO2S</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O9" s="8" t="str">
+        <f>M9</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>71</v>
       </c>
@@ -2260,13 +2273,17 @@
         <f t="shared" si="5"/>
         <v>ENV</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O10" s="8" t="str">
+        <f>M10</f>
+        <v>ENV</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -2317,8 +2334,12 @@
         <f t="shared" si="7"/>
         <v>UP</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O12" s="8" t="str">
+        <f>M12</f>
+        <v>UP</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>79</v>
       </c>
@@ -2369,8 +2390,12 @@
         <f t="shared" si="9"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O13" s="8">
+        <f>M13</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" t="s">
         <v>80</v>
@@ -2422,7 +2447,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O14"/>
+      <c r="O14" s="8">
+        <f>M14</f>
+        <v>1</v>
+      </c>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
@@ -2435,13 +2463,13 @@
       <c r="Y14"/>
       <c r="Z14"/>
       <c r="AA14"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB14"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="M15"/>
-      <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
@@ -2453,13 +2481,13 @@
       <c r="X15"/>
       <c r="Y15"/>
       <c r="Z15"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AA15"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="M16"/>
-      <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
@@ -2471,13 +2499,13 @@
       <c r="X16"/>
       <c r="Y16"/>
       <c r="Z16"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA16"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="M17"/>
-      <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
@@ -2489,6 +2517,7 @@
       <c r="X17"/>
       <c r="Y17"/>
       <c r="Z17"/>
+      <c r="AA17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2498,10 +2527,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,48 +2621,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$O$14,2,FALSE) &amp; "_Single"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$P$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_NetZero_CO2_2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>33792</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$O$14,2,FALSE) &amp; " - Single"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$P$14,2,FALSE) &amp; " - Single"</f>
         <v>Net Zero CO2 by 2050 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
@@ -2641,46 +2670,46 @@
         <v>2020</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>35644</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
@@ -2688,46 +2717,46 @@
         <v>2021</v>
       </c>
       <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F11" s="8">
         <v>2022</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H11" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>36186</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F12" s="8">
@@ -2735,46 +2764,46 @@
         <v>2022</v>
       </c>
       <c r="I12" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F13" s="8">
         <v>2023</v>
       </c>
       <c r="G13" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H13" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>35729</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F14" s="8">
@@ -2782,46 +2811,46 @@
         <v>2023</v>
       </c>
       <c r="I14" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F15" s="8">
         <v>2024</v>
       </c>
       <c r="G15" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H15" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J15" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>31282</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E16" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F16" s="8">
@@ -2829,46 +2858,46 @@
         <v>2024</v>
       </c>
       <c r="I16" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F17" s="8">
         <v>2025</v>
       </c>
       <c r="G17" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H17" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J17" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>27390</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E18" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F18" s="8">
@@ -2876,46 +2905,46 @@
         <v>2025</v>
       </c>
       <c r="I18" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F19" s="8">
         <v>2026</v>
       </c>
       <c r="G19" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H19" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J19" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>23981</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E20" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F20" s="8">
@@ -2923,46 +2952,46 @@
         <v>2026</v>
       </c>
       <c r="I20" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F21" s="8">
         <v>2027</v>
       </c>
       <c r="G21" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H21" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J21" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>20997</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E22" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F22" s="8">
@@ -2970,46 +2999,46 @@
         <v>2027</v>
       </c>
       <c r="I22" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F23" s="8">
         <v>2028</v>
       </c>
       <c r="G23" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H23" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J23" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>18384</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E24" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F24" s="8">
@@ -3017,46 +3046,46 @@
         <v>2028</v>
       </c>
       <c r="I24" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D25" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F25" s="8">
         <v>2029</v>
       </c>
       <c r="G25" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H25" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J25" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>16096</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D26" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E26" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F26" s="8">
@@ -3064,46 +3093,46 @@
         <v>2029</v>
       </c>
       <c r="I26" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D27" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F27" s="8">
         <v>2030</v>
       </c>
       <c r="G27" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H27" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J27" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>14093</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E28" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F28" s="8">
@@ -3111,63 +3140,110 @@
         <v>2030</v>
       </c>
       <c r="I28" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D29" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F29" s="8">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="G29" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H29" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
-      <c r="J29" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>0</v>
+      <c r="J29" s="17">
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
+        <v>13848.092860693008</v>
       </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D30" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E30" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F30" s="8">
         <f>F29</f>
+        <v>2035</v>
+      </c>
+      <c r="I30" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F31" s="8">
         <v>2050</v>
       </c>
-      <c r="I30" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+      <c r="G31" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H31" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E32" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F32" s="8">
+        <f>F31</f>
+        <v>2050</v>
+      </c>
+      <c r="I32" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="8">
+    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="J31" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F31,config!$B$6:$O$6,),FALSE)</f>
+      <c r="J33" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F33,config!$B$6:$P$6,),FALSE)</f>
         <v>5</v>
       </c>
     </row>
@@ -3179,10 +3255,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3273,48 +3349,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$O$14,2,FALSE) &amp; "_Multi"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$P$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_NetZero_CO2_2050_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F7,config!$B$6:$P$6,),FALSE)</f>
         <v>33792</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$O$14,2,FALSE) &amp; " - Multi"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$P$14,2,FALSE) &amp; " - Multi"</f>
         <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
@@ -3322,46 +3398,46 @@
         <v>2020</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F8,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F9,config!$B$6:$P$6,),FALSE)</f>
         <v>35644</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
@@ -3369,46 +3445,46 @@
         <v>2021</v>
       </c>
       <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F10,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F11" s="8">
         <v>2022</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H11" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F11,config!$B$6:$P$6,),FALSE)</f>
         <v>36186</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F12" s="8">
@@ -3416,46 +3492,46 @@
         <v>2022</v>
       </c>
       <c r="I12" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F12,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F13" s="8">
         <v>2023</v>
       </c>
       <c r="G13" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H13" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F13,config!$B$6:$P$6,),FALSE)</f>
         <v>35729</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F14" s="8">
@@ -3463,46 +3539,46 @@
         <v>2023</v>
       </c>
       <c r="I14" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F14,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F15" s="8">
         <v>2024</v>
       </c>
       <c r="G15" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H15" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J15" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F15,config!$B$6:$P$6,),FALSE)</f>
         <v>31282</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E16" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F16" s="8">
@@ -3510,46 +3586,46 @@
         <v>2024</v>
       </c>
       <c r="I16" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F16,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F17" s="8">
         <v>2025</v>
       </c>
       <c r="G17" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H17" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J17" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F17,config!$B$6:$P$6,),FALSE)</f>
         <v>27390</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E18" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F18" s="8">
@@ -3557,46 +3633,46 @@
         <v>2025</v>
       </c>
       <c r="I18" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F18,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F19" s="8">
         <v>2026</v>
       </c>
       <c r="G19" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H19" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J19" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F19,config!$B$6:$P$6,),FALSE)</f>
         <v>23981</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E20" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F20" s="8">
@@ -3604,46 +3680,46 @@
         <v>2026</v>
       </c>
       <c r="I20" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F20,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F21" s="8">
         <v>2027</v>
       </c>
       <c r="G21" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H21" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J21" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F21,config!$B$6:$P$6,),FALSE)</f>
         <v>20997</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E22" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F22" s="8">
@@ -3651,46 +3727,46 @@
         <v>2027</v>
       </c>
       <c r="I22" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F22,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F23" s="8">
         <v>2028</v>
       </c>
       <c r="G23" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H23" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J23" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F23,config!$B$6:$P$6,),FALSE)</f>
         <v>18384</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E24" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F24" s="8">
@@ -3698,46 +3774,46 @@
         <v>2028</v>
       </c>
       <c r="I24" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F24,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D25" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F25" s="8">
         <v>2029</v>
       </c>
       <c r="G25" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H25" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J25" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F25,config!$B$6:$P$6,),FALSE)</f>
         <v>16096</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D26" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E26" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F26" s="8">
@@ -3745,46 +3821,46 @@
         <v>2029</v>
       </c>
       <c r="I26" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F26,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D27" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F27" s="8">
         <v>2030</v>
       </c>
       <c r="G27" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H27" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J27" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F27,config!$B$6:$P$6,),FALSE)</f>
         <v>14093</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E28" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F28" s="8">
@@ -3792,62 +3868,108 @@
         <v>2030</v>
       </c>
       <c r="I28" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F28,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D29" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F29" s="8">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="G29" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H29" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
         <v>1</v>
       </c>
-      <c r="J29" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>0</v>
+      <c r="J29" s="17">
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F29,config!$B$6:$P$6,),FALSE)</f>
+        <v>13848.092860693008</v>
       </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D30" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E30" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F30" s="8">
+        <v>2035</v>
+      </c>
+      <c r="I30" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F30,config!$B$6:$P$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D31" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F31" s="8">
         <v>2050</v>
       </c>
-      <c r="I30" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
+      <c r="G31" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H31" s="8">
+        <f>VLOOKUP(H$5, config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F31,config!$B$6:$P$6,),FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D32" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E32" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F32" s="8">
+        <v>2050</v>
+      </c>
+      <c r="I32" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$P$14,MATCH($F32,config!$B$6:$P$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="8">
+    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="J31" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F31,config!$B$6:$O$6,),FALSE)</f>
+      <c r="J33" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$P$14,MATCH($F33,config!$B$6:$P$6,),FALSE)</f>
         <v>5</v>
       </c>
     </row>

</xml_diff>